<commit_message>
Rename Kerr sample server
</commit_message>
<xml_diff>
--- a/RtdBugExcel2409.xlsx
+++ b/RtdBugExcel2409.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\RtdBugExcel2409\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEFF0C3-E22B-4017-AFB9-D90833BAC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76FB896-11C9-42B5-8E56-90029E949C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="1860" windowWidth="18315" windowHeight="11460" xr2:uid="{1667AB4B-FA20-472D-8A31-EC718DFBCE22}"/>
+    <workbookView xWindow="7365" yWindow="2205" windowWidth="18315" windowHeight="11460" xr2:uid="{1667AB4B-FA20-472D-8A31-EC718DFBCE22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
   <si>
     <t>c</t>
@@ -50,10 +47,10 @@
     <t>h</t>
   </si>
   <si>
-    <t>i</t>
+    <t>j</t>
   </si>
   <si>
-    <t>j</t>
+    <t>dd</t>
   </si>
 </sst>
 </file>
@@ -111,6 +108,22 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
+    <main first="exceldna.rtdserver.slowadd">
+      <tp>
+        <v>3</v>
+        <stp/>
+        <stp>1</stp>
+        <stp>2</stp>
+        <tr r="C1" s="1"/>
+      </tp>
+      <tp>
+        <v>7</v>
+        <stp/>
+        <stp>3</stp>
+        <stp>4</stp>
+        <tr r="C3" s="1"/>
+      </tp>
+    </main>
     <main first="exceldna.rtdserver.slowecho">
       <tp t="s">
         <v>j</v>
@@ -125,18 +138,6 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp t="s">
-        <v>i</v>
-        <stp/>
-        <stp>i</stp>
-        <tr r="H9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>b</v>
-        <stp/>
-        <stp>b</stp>
-        <tr r="H2" s="1"/>
-      </tp>
-      <tp t="s">
         <v>c</v>
         <stp/>
         <stp>c</stp>
@@ -149,44 +150,63 @@
         <tr r="H1" s="1"/>
       </tp>
       <tp t="s">
-        <v>### Delayed ...</v>
+        <v>4</v>
         <stp/>
         <stp>4</stp>
         <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
-        <v>### Delayed ...</v>
+        <v>2</v>
         <stp/>
         <stp>2</stp>
         <tr r="H5" s="1"/>
       </tp>
       <tp t="s">
-        <v>### Delayed ...</v>
-        <stp/>
-        <stp>3</stp>
-        <tr r="H6" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>### Delayed ...</v>
+        <v>1</v>
         <stp/>
         <stp>1</stp>
         <tr r="H4" s="1"/>
       </tp>
+      <tp t="s">
+        <v>### Delayed ...</v>
+        <stp/>
+        <stp>dd</stp>
+        <tr r="H6" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>### Delayed ...</v>
+        <stp/>
+        <stp>77</stp>
+        <tr r="H9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>### Delayed ...</v>
+        <stp/>
+        <stp>12</stp>
+        <tr r="H2" s="1"/>
+      </tp>
     </main>
     <main first="exceldna.rtdserver.slowadd">
       <tp>
-        <v>109</v>
-        <stp/>
-        <stp>10</stp>
+        <v>143</v>
+        <stp/>
+        <stp>44</stp>
+        <stp>99</stp>
+        <tr r="C9" s="1"/>
+      </tp>
+      <tp>
+        <v>144</v>
+        <stp/>
+        <stp>45</stp>
         <stp>99</stp>
         <tr r="C10" s="1"/>
       </tp>
-      <tp>
-        <v>108</v>
-        <stp/>
-        <stp>9</stp>
-        <stp>99</stp>
-        <tr r="C9" s="1"/>
+      <tp t="s">
+        <v>### Delayed ...</v>
+        <stp/>
+        <stp>5</stp>
+        <stp>12</stp>
+        <tr r="C5" s="1"/>
       </tp>
       <tp>
         <v>107</v>
@@ -196,32 +216,11 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>100</v>
-        <stp/>
-        <stp>1</stp>
-        <stp>99</stp>
-        <tr r="C1" s="1"/>
-      </tp>
-      <tp>
-        <v>102</v>
-        <stp/>
-        <stp>3</stp>
-        <stp>99</stp>
-        <tr r="C3" s="1"/>
-      </tp>
-      <tp>
         <v>101</v>
         <stp/>
         <stp>2</stp>
         <stp>99</stp>
         <tr r="C2" s="1"/>
-      </tp>
-      <tp>
-        <v>104</v>
-        <stp/>
-        <stp>5</stp>
-        <stp>99</stp>
-        <tr r="C5" s="1"/>
       </tp>
       <tp>
         <v>103</v>
@@ -569,7 +568,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,11 +578,11 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="C1">
         <f>RTD("exceldna.rtdserver.slowadd",,A1,B1)</f>
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -605,12 +604,12 @@
         <f>RTD("exceldna.rtdserver.slowadd",,A2,B2)</f>
         <v>101</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
+      <c r="G2">
+        <v>12</v>
       </c>
       <c r="H2" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G2)</f>
-        <v>b</v>
+        <v>### Delayed ...</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -619,14 +618,14 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>RTD("exceldna.rtdserver.slowadd",,A3,B3)</f>
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G3)</f>
@@ -650,7 +649,7 @@
       </c>
       <c r="H4" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G4)</f>
-        <v>### Delayed ...</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -659,18 +658,18 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>99</v>
-      </c>
-      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="C5" t="str">
         <f>RTD("exceldna.rtdserver.slowadd",,A5,B5)</f>
-        <v>104</v>
+        <v>### Delayed ...</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G5)</f>
-        <v>### Delayed ...</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,8 +684,8 @@
         <f>RTD("exceldna.rtdserver.slowadd",,A6,B6)</f>
         <v>105</v>
       </c>
-      <c r="G6">
-        <v>3</v>
+      <c r="G6" t="s">
+        <v>4</v>
       </c>
       <c r="H6" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G6)</f>
@@ -710,7 +709,7 @@
       </c>
       <c r="H7" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G7)</f>
-        <v>### Delayed ...</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,7 +725,7 @@
         <v>107</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G8)</f>
@@ -735,38 +734,37 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>99</v>
       </c>
       <c r="C9">
         <f>RTD("exceldna.rtdserver.slowadd",,A9,B9)</f>
-        <v>108</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
+        <v>143</v>
+      </c>
+      <c r="G9">
+        <v>77</v>
       </c>
       <c r="H9" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G9)</f>
-        <v>i</v>
+        <v>### Delayed ...</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>99</v>
       </c>
       <c r="C10">
         <f>RTD("exceldna.rtdserver.slowadd",,A10,B10)</f>
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" t="str">
         <f>RTD("exceldna.rtdserver.slowecho",,G10)</f>

</xml_diff>